<commit_message>
updated excel reading condition
</commit_message>
<xml_diff>
--- a/src/main/java/Data/EcomData.xlsx
+++ b/src/main/java/Data/EcomData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub public repo\PreethiSri-Selenium-Java-Project\src\main\java\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD697FA4-D861-41B5-A6C0-44C634C8D671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADFD7A3-3499-45D3-8745-88F328695883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4DBE2160-5AD7-4909-81B6-FF930011E616}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Category</t>
   </si>
@@ -52,15 +52,6 @@
   </si>
   <si>
     <t>Phone</t>
-  </si>
-  <si>
-    <t>iphone</t>
-  </si>
-  <si>
-    <t>laptop</t>
-  </si>
-  <si>
-    <t>samsung</t>
   </si>
   <si>
     <t>Latitude</t>
@@ -109,7 +100,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +118,14 @@
       <color rgb="FF080808"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -144,19 +143,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -493,45 +511,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D47143F-35AA-42B1-B582-FD72C3217BE6}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -543,7 +549,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="G12" activeCellId="1" sqref="A1:F4 G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -553,83 +559,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>-10.457800000000001</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="4">
         <v>12.7887</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>-20.124300000000002</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="4">
         <v>21.321999999999999</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2">
+      <c r="A4" s="4">
         <v>-2.7833000000000001</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>8.5640000000000001</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>4</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
API added validation for getAPI,class for deserialization class
</commit_message>
<xml_diff>
--- a/src/main/java/Data/EcomData.xlsx
+++ b/src/main/java/Data/EcomData.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub public repo\PreethiSri-Selenium-Java-Project\src\main\java\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADFD7A3-3499-45D3-8745-88F328695883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AAADBE1-F7EF-4AA8-AF99-8AA5EB87EEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4DBE2160-5AD7-4909-81B6-FF930011E616}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{4DBE2160-5AD7-4909-81B6-FF930011E616}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoBlaze" sheetId="1" r:id="rId1"/>
     <sheet name="APIData" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,22 +51,31 @@
     <t>Apple monitor 24</t>
   </si>
   <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Accuacy</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Phone</t>
   </si>
   <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Accuacy</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Street</t>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>language</t>
   </si>
   <si>
     <t>Residency A</t>
@@ -75,25 +84,16 @@
     <t>(+61) 767 444 4444</t>
   </si>
   <si>
-    <t>Residency B</t>
-  </si>
-  <si>
-    <t>Residency C</t>
-  </si>
-  <si>
-    <t>(+61) 1214 5789</t>
-  </si>
-  <si>
-    <t>(+61) 1547 4586</t>
-  </si>
-  <si>
-    <t>Ranson street</t>
-  </si>
-  <si>
     <t>Murray street</t>
   </si>
   <si>
-    <t>Stephen</t>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>http://google.com</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -135,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -158,11 +158,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -171,10 +186,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -517,7 +534,7 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
@@ -546,98 +563,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37703F9-3868-4C9D-89DE-80BEA00C209B}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" activeCellId="1" sqref="A1:F4 G12"/>
+      <selection sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4">
+    <row r="2" spans="1:9" ht="15">
+      <c r="A2" s="6">
         <v>-10.457800000000001</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="6">
         <v>12.7887</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="7">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="I2" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4">
-        <v>-20.124300000000002</v>
-      </c>
-      <c r="B3" s="4">
-        <v>21.321999999999999</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4">
-        <v>-2.7833000000000001</v>
-      </c>
-      <c r="B4" s="4">
-        <v>8.5640000000000001</v>
-      </c>
-      <c r="C4" s="5">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
+    <row r="3" spans="1:9" ht="15"/>
+    <row r="4" spans="1:9" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>